<commit_message>
:bug: Add datetime column to irradiance frames
</commit_message>
<xml_diff>
--- a/outputs/mpp_daily_summary_circular_polysolar_kent.xlsx
+++ b/outputs/mpp_daily_summary_circular_polysolar_kent.xlsx
@@ -522,7 +522,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>73.58474993502155</v>
+        <v>73.58474993502153</v>
       </c>
     </row>
     <row r="12">
@@ -546,7 +546,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>109.2771634057628</v>
+        <v>109.2771634057627</v>
       </c>
     </row>
     <row r="15">
@@ -554,7 +554,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>87.96340703366516</v>
+        <v>87.96340703366513</v>
       </c>
     </row>
     <row r="16">
@@ -644,7 +644,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>571.4412635417107</v>
+        <v>571.4412635417104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>